<commit_message>
figures and multipanel figure update
</commit_message>
<xml_diff>
--- a/figures/heatmap.xlsx
+++ b/figures/heatmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Desktop/Review_figures/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9F0F8F-C35F-9E41-947E-1A1E5DB9BAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA18084-48E6-4545-99DA-3FE51ECD30BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="760" windowWidth="27640" windowHeight="15660" activeTab="5" xr2:uid="{A9C2CF92-978C-AA41-BFCE-FA732D293089}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="115">
   <si>
     <t>Disease</t>
   </si>
@@ -379,6 +379,9 @@
   <si>
     <t>Microbial DNA isolation methods</t>
   </si>
+  <si>
+    <t>DIAMOND</t>
+  </si>
 </sst>
 </file>
 
@@ -686,24 +689,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -788,6 +773,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,46 +1108,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB1AA5-BB65-0E47-B263-AF583DABF612}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="66" workbookViewId="0">
+    <sheetView zoomScale="66" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33" t="s">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
     </row>
     <row r="2" spans="1:24" ht="221" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
+      <c r="A2" s="61"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2619,7 +2622,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+      <selection sqref="A1:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2631,33 +2634,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="6" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="36" t="s">
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="37"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="66"/>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="134" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="64"/>
       <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
@@ -2904,7 +2907,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
@@ -3486,10 +3489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCC52DF-2861-C943-AFB3-5B2E48A96220}">
-  <dimension ref="A1:BD32"/>
+  <dimension ref="A1:BE33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="110" workbookViewId="0">
-      <selection activeCell="AL42" sqref="AL42"/>
+    <sheetView topLeftCell="A7" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3504,7 +3507,7 @@
     <col min="56" max="56" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3670,15 +3673,18 @@
       <c r="BD1" t="s">
         <v>98</v>
       </c>
+      <c r="BE1" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <f t="shared" ref="A3:A31" si="0">SUM(C3:BD3)</f>
+        <f t="shared" ref="A3:A32" si="0">SUM(C3:BD3)</f>
         <v>3</v>
       </c>
       <c r="B3">
@@ -3846,8 +3852,11 @@
       <c r="BD3">
         <v>0</v>
       </c>
+      <c r="BE3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4017,8 +4026,11 @@
       <c r="BD4">
         <v>0</v>
       </c>
+      <c r="BE4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4188,8 +4200,11 @@
       <c r="BD5">
         <v>0</v>
       </c>
+      <c r="BE5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4359,8 +4374,11 @@
       <c r="BD6">
         <v>0</v>
       </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4530,8 +4548,11 @@
       <c r="BD7">
         <v>0</v>
       </c>
+      <c r="BE7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4701,8 +4722,11 @@
       <c r="BD8">
         <v>0</v>
       </c>
+      <c r="BE8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4872,8 +4896,11 @@
       <c r="BD9">
         <v>0</v>
       </c>
+      <c r="BE9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5043,8 +5070,11 @@
       <c r="BD10">
         <v>0</v>
       </c>
+      <c r="BE10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5214,8 +5244,11 @@
       <c r="BD11">
         <v>0</v>
       </c>
+      <c r="BE11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5385,8 +5418,11 @@
       <c r="BD12">
         <v>0</v>
       </c>
+      <c r="BE12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5556,8 +5592,11 @@
       <c r="BD13">
         <v>0</v>
       </c>
+      <c r="BE13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5727,8 +5766,11 @@
       <c r="BD14">
         <v>0</v>
       </c>
+      <c r="BE14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5898,8 +5940,11 @@
       <c r="BD15">
         <v>0</v>
       </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -6069,8 +6114,11 @@
       <c r="BD16">
         <v>0</v>
       </c>
+      <c r="BE16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6240,8 +6288,11 @@
       <c r="BD17">
         <v>0</v>
       </c>
+      <c r="BE17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -6411,8 +6462,11 @@
       <c r="BD18">
         <v>0</v>
       </c>
+      <c r="BE18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -6582,8 +6636,11 @@
       <c r="BD19">
         <v>0</v>
       </c>
+      <c r="BE19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -6753,8 +6810,11 @@
       <c r="BD20">
         <v>0</v>
       </c>
+      <c r="BE20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6924,8 +6984,11 @@
       <c r="BD21">
         <v>0</v>
       </c>
+      <c r="BE21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7095,8 +7158,11 @@
       <c r="BD22">
         <v>0</v>
       </c>
+      <c r="BE22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7266,8 +7332,11 @@
       <c r="BD23">
         <v>0</v>
       </c>
+      <c r="BE23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7437,8 +7506,11 @@
       <c r="BD24">
         <v>0</v>
       </c>
+      <c r="BE24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7608,8 +7680,11 @@
       <c r="BD25">
         <v>0</v>
       </c>
+      <c r="BE25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7779,8 +7854,11 @@
       <c r="BD26">
         <v>0</v>
       </c>
+      <c r="BE26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7950,8 +8028,11 @@
       <c r="BD27">
         <v>0</v>
       </c>
+      <c r="BE27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8121,8 +8202,11 @@
       <c r="BD28">
         <v>1</v>
       </c>
+      <c r="BE28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8292,8 +8376,11 @@
       <c r="BD29">
         <v>0</v>
       </c>
+      <c r="BE29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -8463,10 +8550,12 @@
       <c r="BD30">
         <v>0</v>
       </c>
+      <c r="BE30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B31">
@@ -8634,233 +8723,427 @@
       <c r="BD31">
         <v>0</v>
       </c>
+      <c r="BE31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:56" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="5">
-        <f>SUM(C3:C31)</f>
-        <v>9</v>
-      </c>
-      <c r="D32" s="5">
-        <f t="shared" ref="D32:BD32" si="1">SUM(D3:D31)</f>
+    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <f>SUM(C32:BE32)</f>
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>0</v>
+      </c>
+      <c r="AN32">
+        <v>0</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>0</v>
+      </c>
+      <c r="AQ32">
+        <v>0</v>
+      </c>
+      <c r="AR32">
+        <v>0</v>
+      </c>
+      <c r="AS32">
+        <v>0</v>
+      </c>
+      <c r="AT32">
+        <v>0</v>
+      </c>
+      <c r="AU32">
+        <v>0</v>
+      </c>
+      <c r="AV32">
+        <v>0</v>
+      </c>
+      <c r="AW32">
+        <v>0</v>
+      </c>
+      <c r="AX32">
+        <v>0</v>
+      </c>
+      <c r="AY32">
+        <v>0</v>
+      </c>
+      <c r="AZ32">
+        <v>0</v>
+      </c>
+      <c r="BA32">
+        <v>0</v>
+      </c>
+      <c r="BB32">
+        <v>0</v>
+      </c>
+      <c r="BC32">
+        <v>0</v>
+      </c>
+      <c r="BD32">
+        <v>0</v>
+      </c>
+      <c r="BE32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:57" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="5">
+        <f>SUM(C3:C32)</f>
+        <v>10</v>
+      </c>
+      <c r="D33" s="5">
+        <f>SUM(D3:D32)</f>
         <v>7</v>
       </c>
-      <c r="E32" s="5">
-        <f t="shared" si="1"/>
+      <c r="E33" s="5">
+        <f>SUM(E3:E32)</f>
         <v>6</v>
       </c>
-      <c r="F32" s="5">
-        <f t="shared" si="1"/>
+      <c r="F33" s="5">
+        <f>SUM(F3:F32)</f>
         <v>6</v>
       </c>
-      <c r="G32" s="5">
-        <f t="shared" si="1"/>
+      <c r="G33" s="5">
+        <f>SUM(G3:G32)</f>
         <v>6</v>
       </c>
-      <c r="H32" s="5">
-        <f t="shared" si="1"/>
+      <c r="H33" s="5">
+        <f>SUM(H3:H32)</f>
         <v>4</v>
       </c>
-      <c r="I32" s="5">
-        <f t="shared" si="1"/>
+      <c r="I33" s="5">
+        <f>SUM(I3:I32)</f>
         <v>4</v>
       </c>
-      <c r="J32" s="5">
-        <f t="shared" si="1"/>
+      <c r="J33" s="5">
+        <f>SUM(J3:J32)</f>
         <v>3</v>
       </c>
-      <c r="K32" s="5">
-        <f t="shared" si="1"/>
+      <c r="K33" s="5">
+        <f>SUM(K3:K32)</f>
         <v>2</v>
       </c>
-      <c r="L32" s="5">
-        <f t="shared" si="1"/>
+      <c r="L33" s="5">
+        <f>SUM(L3:L32)</f>
         <v>2</v>
       </c>
-      <c r="M32" s="5">
-        <f t="shared" si="1"/>
+      <c r="M33" s="5">
+        <f>SUM(M3:M32)</f>
         <v>2</v>
       </c>
-      <c r="N32" s="5">
-        <f t="shared" si="1"/>
+      <c r="N33" s="5">
+        <f>SUM(N3:N32)</f>
         <v>2</v>
       </c>
-      <c r="O32" s="5">
-        <f t="shared" si="1"/>
+      <c r="O33" s="5">
+        <f>SUM(O3:O32)</f>
         <v>2</v>
       </c>
-      <c r="P32" s="5">
-        <f t="shared" si="1"/>
+      <c r="P33" s="5">
+        <f>SUM(P3:P32)</f>
         <v>2</v>
       </c>
-      <c r="Q32" s="5">
-        <f t="shared" si="1"/>
+      <c r="Q33" s="5">
+        <f>SUM(Q3:Q32)</f>
         <v>2</v>
       </c>
-      <c r="R32" s="5">
-        <f t="shared" si="1"/>
+      <c r="R33" s="5">
+        <f>SUM(R3:R32)</f>
         <v>2</v>
       </c>
-      <c r="S32" s="5">
-        <f t="shared" si="1"/>
+      <c r="S33" s="5">
+        <f>SUM(S3:S32)</f>
         <v>2</v>
       </c>
-      <c r="T32" s="5">
-        <f t="shared" si="1"/>
+      <c r="T33" s="5">
+        <f>SUM(T3:T32)</f>
         <v>2</v>
       </c>
-      <c r="U32" s="5">
-        <f t="shared" si="1"/>
+      <c r="U33" s="5">
+        <f>SUM(U3:U32)</f>
         <v>2</v>
       </c>
-      <c r="V32" s="5">
-        <f t="shared" si="1"/>
+      <c r="V33" s="5">
+        <f>SUM(V3:V32)</f>
         <v>2</v>
       </c>
-      <c r="W32" s="5">
-        <f t="shared" si="1"/>
+      <c r="W33" s="5">
+        <f>SUM(W3:W32)</f>
         <v>2</v>
       </c>
-      <c r="X32" s="5">
-        <f t="shared" si="1"/>
+      <c r="X33" s="5">
+        <f>SUM(X3:X32)</f>
         <v>2</v>
       </c>
-      <c r="Y32" s="5">
-        <f t="shared" si="1"/>
+      <c r="Y33" s="5">
+        <f>SUM(Y3:Y32)</f>
         <v>2</v>
       </c>
-      <c r="Z32" s="5">
-        <f t="shared" si="1"/>
+      <c r="Z33" s="5">
+        <f>SUM(Z3:Z32)</f>
         <v>2</v>
       </c>
-      <c r="AA32" s="5">
-        <f t="shared" si="1"/>
+      <c r="AA33" s="5">
+        <f>SUM(AA3:AA32)</f>
         <v>2</v>
       </c>
-      <c r="AB32" s="5">
-        <f t="shared" si="1"/>
+      <c r="AB33" s="5">
+        <f>SUM(AB3:AB32)</f>
         <v>2</v>
       </c>
-      <c r="AC32" s="5">
-        <f t="shared" si="1"/>
+      <c r="AC33" s="5">
+        <f>SUM(AC3:AC32)</f>
         <v>2</v>
       </c>
-      <c r="AD32" s="5">
-        <f t="shared" si="1"/>
+      <c r="AD33" s="5">
+        <f>SUM(AD3:AD32)</f>
         <v>2</v>
       </c>
-      <c r="AE32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AF32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AG32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AH32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AI32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AJ32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AK32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AL32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AM32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AN32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AO32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AP32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AQ32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AR32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AS32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AT32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AU32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AV32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AW32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AX32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AY32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AZ32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BA32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BB32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BC32" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BD32" s="5">
-        <f t="shared" si="1"/>
+      <c r="AE33" s="5">
+        <f>SUM(AE3:AE32)</f>
+        <v>1</v>
+      </c>
+      <c r="AF33" s="5">
+        <f>SUM(AF3:AF32)</f>
+        <v>1</v>
+      </c>
+      <c r="AG33" s="5">
+        <f>SUM(AG3:AG32)</f>
+        <v>1</v>
+      </c>
+      <c r="AH33" s="5">
+        <f>SUM(AH3:AH32)</f>
+        <v>1</v>
+      </c>
+      <c r="AI33" s="5">
+        <f>SUM(AI3:AI32)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="5">
+        <f>SUM(AJ3:AJ32)</f>
+        <v>1</v>
+      </c>
+      <c r="AK33" s="5">
+        <f>SUM(AK3:AK32)</f>
+        <v>1</v>
+      </c>
+      <c r="AL33" s="5">
+        <f>SUM(AL3:AL32)</f>
+        <v>1</v>
+      </c>
+      <c r="AM33" s="5">
+        <f>SUM(AM3:AM32)</f>
+        <v>1</v>
+      </c>
+      <c r="AN33" s="5">
+        <f>SUM(AN3:AN32)</f>
+        <v>1</v>
+      </c>
+      <c r="AO33" s="5">
+        <f>SUM(AO3:AO32)</f>
+        <v>1</v>
+      </c>
+      <c r="AP33" s="5">
+        <f>SUM(AP3:AP32)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ33" s="5">
+        <f>SUM(AQ3:AQ32)</f>
+        <v>1</v>
+      </c>
+      <c r="AR33" s="5">
+        <f>SUM(AR3:AR32)</f>
+        <v>1</v>
+      </c>
+      <c r="AS33" s="5">
+        <f>SUM(AS3:AS32)</f>
+        <v>1</v>
+      </c>
+      <c r="AT33" s="5">
+        <f>SUM(AT3:AT32)</f>
+        <v>1</v>
+      </c>
+      <c r="AU33" s="5">
+        <f>SUM(AU3:AU32)</f>
+        <v>1</v>
+      </c>
+      <c r="AV33" s="5">
+        <f>SUM(AV3:AV32)</f>
+        <v>1</v>
+      </c>
+      <c r="AW33" s="5">
+        <f>SUM(AW3:AW32)</f>
+        <v>1</v>
+      </c>
+      <c r="AX33" s="5">
+        <f>SUM(AX3:AX32)</f>
+        <v>1</v>
+      </c>
+      <c r="AY33" s="5">
+        <f>SUM(AY3:AY32)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ33" s="5">
+        <f>SUM(AZ3:AZ32)</f>
+        <v>1</v>
+      </c>
+      <c r="BA33" s="5">
+        <f>SUM(BA3:BA32)</f>
+        <v>1</v>
+      </c>
+      <c r="BB33" s="5">
+        <f>SUM(BB3:BB32)</f>
+        <v>1</v>
+      </c>
+      <c r="BC33" s="5">
+        <f>SUM(BC3:BC32)</f>
+        <v>1</v>
+      </c>
+      <c r="BD33" s="5">
+        <f>SUM(BD3:BD32)</f>
+        <v>1</v>
+      </c>
+      <c r="BE33" s="5">
+        <f>SUM(BE3:BE32)</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:BD31">
-    <cfRule type="colorScale" priority="184">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:BE33">
+    <sortCondition ref="B3"/>
+  </sortState>
+  <conditionalFormatting sqref="C3:BE32">
+    <cfRule type="colorScale" priority="185">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:A32">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -8871,16 +9154,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5052CE14-51AE-A345-AB4E-33AAF1D2E60B}">
-  <dimension ref="A1:AC31"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:AC15"/>
+      <selection sqref="A1:AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="29" width="6.83203125" customWidth="1"/>
+    <col min="2" max="4" width="6.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="9" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="20" width="6.83203125" customWidth="1"/>
+    <col min="21" max="21" width="7.33203125" customWidth="1"/>
+    <col min="22" max="29" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -11498,96 +11789,188 @@
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A31" s="29">
+      <c r="A31" s="28">
         <v>28</v>
       </c>
-      <c r="B31" s="30">
-        <v>0</v>
-      </c>
-      <c r="C31" s="30">
-        <v>0</v>
-      </c>
-      <c r="D31" s="30">
-        <v>0</v>
-      </c>
-      <c r="E31" s="30">
-        <v>0</v>
-      </c>
-      <c r="F31" s="30">
-        <v>0</v>
-      </c>
-      <c r="G31" s="30">
-        <v>0</v>
-      </c>
-      <c r="H31" s="30">
-        <v>0</v>
-      </c>
-      <c r="I31" s="30">
-        <v>0</v>
-      </c>
-      <c r="J31" s="30">
-        <v>0</v>
-      </c>
-      <c r="K31" s="30">
-        <v>0</v>
-      </c>
-      <c r="L31" s="30">
-        <v>0</v>
-      </c>
-      <c r="M31" s="30">
-        <v>1</v>
-      </c>
-      <c r="N31" s="30">
-        <v>1</v>
-      </c>
-      <c r="O31" s="30">
-        <v>0</v>
-      </c>
-      <c r="P31" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="30">
-        <v>0</v>
-      </c>
-      <c r="R31" s="30">
-        <v>0</v>
-      </c>
-      <c r="S31" s="30">
-        <v>0</v>
-      </c>
-      <c r="T31" s="30">
-        <v>0</v>
-      </c>
-      <c r="U31" s="30">
-        <v>0</v>
-      </c>
-      <c r="V31" s="30">
-        <v>0</v>
-      </c>
-      <c r="W31" s="30">
-        <v>0</v>
-      </c>
-      <c r="X31" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="30">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="31">
+      <c r="B31" s="26">
+        <v>0</v>
+      </c>
+      <c r="C31" s="26">
+        <v>0</v>
+      </c>
+      <c r="D31" s="26">
+        <v>0</v>
+      </c>
+      <c r="E31" s="26">
+        <v>0</v>
+      </c>
+      <c r="F31" s="26">
+        <v>0</v>
+      </c>
+      <c r="G31" s="26">
+        <v>0</v>
+      </c>
+      <c r="H31" s="26">
+        <v>0</v>
+      </c>
+      <c r="I31" s="26">
+        <v>0</v>
+      </c>
+      <c r="J31" s="26">
+        <v>0</v>
+      </c>
+      <c r="K31" s="26">
+        <v>0</v>
+      </c>
+      <c r="L31" s="26">
+        <v>0</v>
+      </c>
+      <c r="M31" s="26">
+        <v>1</v>
+      </c>
+      <c r="N31" s="26">
+        <v>1</v>
+      </c>
+      <c r="O31" s="26">
+        <v>0</v>
+      </c>
+      <c r="P31" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="26">
+        <v>0</v>
+      </c>
+      <c r="R31" s="26">
+        <v>0</v>
+      </c>
+      <c r="S31" s="26">
+        <v>0</v>
+      </c>
+      <c r="T31" s="26">
+        <v>0</v>
+      </c>
+      <c r="U31" s="26">
+        <v>0</v>
+      </c>
+      <c r="V31" s="26">
+        <v>0</v>
+      </c>
+      <c r="W31" s="26">
+        <v>0</v>
+      </c>
+      <c r="X31" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A32" s="29">
+        <v>29</v>
+      </c>
+      <c r="B32" s="30">
+        <v>1</v>
+      </c>
+      <c r="C32" s="30">
+        <v>0</v>
+      </c>
+      <c r="D32" s="30">
+        <v>0</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="30">
+        <v>0</v>
+      </c>
+      <c r="G32" s="30">
+        <v>0</v>
+      </c>
+      <c r="H32" s="30">
+        <v>0</v>
+      </c>
+      <c r="I32" s="30">
+        <v>0</v>
+      </c>
+      <c r="J32" s="30">
+        <v>0</v>
+      </c>
+      <c r="K32" s="30">
+        <v>0</v>
+      </c>
+      <c r="L32" s="30">
+        <v>0</v>
+      </c>
+      <c r="M32" s="30">
+        <v>0</v>
+      </c>
+      <c r="N32" s="30">
+        <v>0</v>
+      </c>
+      <c r="O32" s="30">
+        <v>0</v>
+      </c>
+      <c r="P32" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="30">
+        <v>0</v>
+      </c>
+      <c r="R32" s="30">
+        <v>0</v>
+      </c>
+      <c r="S32" s="30">
+        <v>0</v>
+      </c>
+      <c r="T32" s="30">
+        <v>0</v>
+      </c>
+      <c r="U32" s="30">
+        <v>0</v>
+      </c>
+      <c r="V32" s="30">
+        <v>0</v>
+      </c>
+      <c r="W32" s="30">
+        <v>0</v>
+      </c>
+      <c r="X32" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="31">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:AC31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AC32">
+    <sortCondition ref="A3"/>
+  </sortState>
+  <conditionalFormatting sqref="B3:AC32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -11607,101 +11990,105 @@
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+      <selection sqref="A1:AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="29" width="6.83203125" customWidth="1"/>
+    <col min="2" max="9" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="20" width="6.83203125" customWidth="1"/>
+    <col min="21" max="21" width="8" customWidth="1"/>
+    <col min="22" max="29" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="55" t="s">
+      <c r="N1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="55" t="s">
+      <c r="O1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="55" t="s">
+      <c r="P1" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="Q1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="T1" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="55" t="s">
+      <c r="U1" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="V1" s="55" t="s">
+      <c r="V1" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="55" t="s">
+      <c r="W1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="X1" s="55" t="s">
+      <c r="X1" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="Y1" s="55" t="s">
+      <c r="Y1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="55" t="s">
+      <c r="Z1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="55" t="s">
+      <c r="AA1" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="55" t="s">
+      <c r="AB1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="56" t="s">
+      <c r="AC1" s="50" t="s">
         <v>73</v>
       </c>
     </row>
@@ -11709,7 +12096,7 @@
       <c r="A2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -11742,88 +12129,88 @@
       <c r="A3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="43">
-        <v>1</v>
-      </c>
-      <c r="C3" s="38">
+      <c r="B3" s="37">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32">
         <v>2</v>
       </c>
-      <c r="D3" s="38">
-        <v>0</v>
-      </c>
-      <c r="E3" s="38">
-        <v>0</v>
-      </c>
-      <c r="F3" s="38">
-        <v>1</v>
-      </c>
-      <c r="G3" s="38">
-        <v>0</v>
-      </c>
-      <c r="H3" s="38">
-        <v>0</v>
-      </c>
-      <c r="I3" s="38">
+      <c r="D3" s="32">
+        <v>0</v>
+      </c>
+      <c r="E3" s="32">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32">
+        <v>1</v>
+      </c>
+      <c r="G3" s="32">
+        <v>0</v>
+      </c>
+      <c r="H3" s="32">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32">
         <v>2</v>
       </c>
-      <c r="J3" s="38">
-        <v>0</v>
-      </c>
-      <c r="K3" s="38">
-        <v>0</v>
-      </c>
-      <c r="L3" s="38">
-        <v>1</v>
-      </c>
-      <c r="M3" s="38">
-        <v>0</v>
-      </c>
-      <c r="N3" s="38">
-        <v>0</v>
-      </c>
-      <c r="O3" s="38">
-        <v>0</v>
-      </c>
-      <c r="P3" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="38">
-        <v>0</v>
-      </c>
-      <c r="R3" s="38">
-        <v>0</v>
-      </c>
-      <c r="S3" s="38">
-        <v>0</v>
-      </c>
-      <c r="T3" s="38">
-        <v>1</v>
-      </c>
-      <c r="U3" s="38">
-        <v>1</v>
-      </c>
-      <c r="V3" s="38">
-        <v>0</v>
-      </c>
-      <c r="W3" s="38">
-        <v>0</v>
-      </c>
-      <c r="X3" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="39">
+      <c r="J3" s="32">
+        <v>0</v>
+      </c>
+      <c r="K3" s="32">
+        <v>0</v>
+      </c>
+      <c r="L3" s="32">
+        <v>1</v>
+      </c>
+      <c r="M3" s="32">
+        <v>0</v>
+      </c>
+      <c r="N3" s="32">
+        <v>0</v>
+      </c>
+      <c r="O3" s="32">
+        <v>0</v>
+      </c>
+      <c r="P3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="32">
+        <v>0</v>
+      </c>
+      <c r="R3" s="32">
+        <v>0</v>
+      </c>
+      <c r="S3" s="32">
+        <v>0</v>
+      </c>
+      <c r="T3" s="32">
+        <v>1</v>
+      </c>
+      <c r="U3" s="32">
+        <v>1</v>
+      </c>
+      <c r="V3" s="32">
+        <v>0</v>
+      </c>
+      <c r="W3" s="32">
+        <v>0</v>
+      </c>
+      <c r="X3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="33">
         <v>0</v>
       </c>
     </row>
@@ -11831,88 +12218,88 @@
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="43">
-        <v>0</v>
-      </c>
-      <c r="C4" s="38">
-        <v>0</v>
-      </c>
-      <c r="D4" s="38">
-        <v>0</v>
-      </c>
-      <c r="E4" s="38">
-        <v>0</v>
-      </c>
-      <c r="F4" s="38">
-        <v>0</v>
-      </c>
-      <c r="G4" s="38">
-        <v>1</v>
-      </c>
-      <c r="H4" s="38">
-        <v>0</v>
-      </c>
-      <c r="I4" s="38">
-        <v>0</v>
-      </c>
-      <c r="J4" s="38">
-        <v>0</v>
-      </c>
-      <c r="K4" s="38">
-        <v>0</v>
-      </c>
-      <c r="L4" s="38">
-        <v>0</v>
-      </c>
-      <c r="M4" s="38">
-        <v>0</v>
-      </c>
-      <c r="N4" s="38">
-        <v>0</v>
-      </c>
-      <c r="O4" s="38">
-        <v>0</v>
-      </c>
-      <c r="P4" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="38">
-        <v>0</v>
-      </c>
-      <c r="R4" s="38">
-        <v>0</v>
-      </c>
-      <c r="S4" s="38">
-        <v>0</v>
-      </c>
-      <c r="T4" s="38">
-        <v>0</v>
-      </c>
-      <c r="U4" s="38">
-        <v>0</v>
-      </c>
-      <c r="V4" s="38">
-        <v>0</v>
-      </c>
-      <c r="W4" s="38">
-        <v>0</v>
-      </c>
-      <c r="X4" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="39">
+      <c r="B4" s="37">
+        <v>0</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0</v>
+      </c>
+      <c r="G4" s="32">
+        <v>1</v>
+      </c>
+      <c r="H4" s="32">
+        <v>0</v>
+      </c>
+      <c r="I4" s="32">
+        <v>0</v>
+      </c>
+      <c r="J4" s="32">
+        <v>0</v>
+      </c>
+      <c r="K4" s="32">
+        <v>0</v>
+      </c>
+      <c r="L4" s="32">
+        <v>0</v>
+      </c>
+      <c r="M4" s="32">
+        <v>0</v>
+      </c>
+      <c r="N4" s="32">
+        <v>0</v>
+      </c>
+      <c r="O4" s="32">
+        <v>0</v>
+      </c>
+      <c r="P4" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>0</v>
+      </c>
+      <c r="R4" s="32">
+        <v>0</v>
+      </c>
+      <c r="S4" s="32">
+        <v>0</v>
+      </c>
+      <c r="T4" s="32">
+        <v>0</v>
+      </c>
+      <c r="U4" s="32">
+        <v>0</v>
+      </c>
+      <c r="V4" s="32">
+        <v>0</v>
+      </c>
+      <c r="W4" s="32">
+        <v>0</v>
+      </c>
+      <c r="X4" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="33">
         <v>0</v>
       </c>
     </row>
@@ -11920,88 +12307,88 @@
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="43">
-        <v>0</v>
-      </c>
-      <c r="C5" s="38">
-        <v>1</v>
-      </c>
-      <c r="D5" s="38">
-        <v>1</v>
-      </c>
-      <c r="E5" s="38">
-        <v>1</v>
-      </c>
-      <c r="F5" s="38">
-        <v>0</v>
-      </c>
-      <c r="G5" s="38">
-        <v>0</v>
-      </c>
-      <c r="H5" s="38">
-        <v>0</v>
-      </c>
-      <c r="I5" s="38">
-        <v>0</v>
-      </c>
-      <c r="J5" s="38">
-        <v>0</v>
-      </c>
-      <c r="K5" s="38">
-        <v>0</v>
-      </c>
-      <c r="L5" s="38">
-        <v>0</v>
-      </c>
-      <c r="M5" s="38">
-        <v>0</v>
-      </c>
-      <c r="N5" s="38">
-        <v>0</v>
-      </c>
-      <c r="O5" s="38">
-        <v>0</v>
-      </c>
-      <c r="P5" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="38">
-        <v>0</v>
-      </c>
-      <c r="R5" s="38">
-        <v>0</v>
-      </c>
-      <c r="S5" s="38">
-        <v>0</v>
-      </c>
-      <c r="T5" s="38">
-        <v>0</v>
-      </c>
-      <c r="U5" s="38">
-        <v>0</v>
-      </c>
-      <c r="V5" s="38">
-        <v>0</v>
-      </c>
-      <c r="W5" s="38">
-        <v>0</v>
-      </c>
-      <c r="X5" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="39">
+      <c r="B5" s="37">
+        <v>0</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1</v>
+      </c>
+      <c r="D5" s="32">
+        <v>1</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32">
+        <v>0</v>
+      </c>
+      <c r="G5" s="32">
+        <v>0</v>
+      </c>
+      <c r="H5" s="32">
+        <v>0</v>
+      </c>
+      <c r="I5" s="32">
+        <v>0</v>
+      </c>
+      <c r="J5" s="32">
+        <v>0</v>
+      </c>
+      <c r="K5" s="32">
+        <v>0</v>
+      </c>
+      <c r="L5" s="32">
+        <v>0</v>
+      </c>
+      <c r="M5" s="32">
+        <v>0</v>
+      </c>
+      <c r="N5" s="32">
+        <v>0</v>
+      </c>
+      <c r="O5" s="32">
+        <v>0</v>
+      </c>
+      <c r="P5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="32">
+        <v>0</v>
+      </c>
+      <c r="R5" s="32">
+        <v>0</v>
+      </c>
+      <c r="S5" s="32">
+        <v>0</v>
+      </c>
+      <c r="T5" s="32">
+        <v>0</v>
+      </c>
+      <c r="U5" s="32">
+        <v>0</v>
+      </c>
+      <c r="V5" s="32">
+        <v>0</v>
+      </c>
+      <c r="W5" s="32">
+        <v>0</v>
+      </c>
+      <c r="X5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="33">
         <v>0</v>
       </c>
     </row>
@@ -12009,88 +12396,88 @@
       <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="43">
-        <v>1</v>
-      </c>
-      <c r="C6" s="38">
-        <v>1</v>
-      </c>
-      <c r="D6" s="38">
-        <v>1</v>
-      </c>
-      <c r="E6" s="38">
+      <c r="B6" s="37">
+        <v>2</v>
+      </c>
+      <c r="C6" s="32">
+        <v>1</v>
+      </c>
+      <c r="D6" s="32">
+        <v>1</v>
+      </c>
+      <c r="E6" s="32">
         <v>5</v>
       </c>
-      <c r="F6" s="38">
-        <v>1</v>
-      </c>
-      <c r="G6" s="38">
-        <v>0</v>
-      </c>
-      <c r="H6" s="38">
-        <v>0</v>
-      </c>
-      <c r="I6" s="38">
-        <v>0</v>
-      </c>
-      <c r="J6" s="38">
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
+      <c r="G6" s="32">
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0</v>
+      </c>
+      <c r="I6" s="32">
+        <v>0</v>
+      </c>
+      <c r="J6" s="32">
         <v>2</v>
       </c>
-      <c r="K6" s="38">
-        <v>0</v>
-      </c>
-      <c r="L6" s="38">
-        <v>0</v>
-      </c>
-      <c r="M6" s="38">
-        <v>0</v>
-      </c>
-      <c r="N6" s="38">
-        <v>0</v>
-      </c>
-      <c r="O6" s="38">
-        <v>0</v>
-      </c>
-      <c r="P6" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="38">
+      <c r="K6" s="32">
+        <v>0</v>
+      </c>
+      <c r="L6" s="32">
+        <v>0</v>
+      </c>
+      <c r="M6" s="32">
+        <v>0</v>
+      </c>
+      <c r="N6" s="32">
+        <v>0</v>
+      </c>
+      <c r="O6" s="32">
+        <v>0</v>
+      </c>
+      <c r="P6" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="32">
         <v>2</v>
       </c>
-      <c r="R6" s="38">
-        <v>0</v>
-      </c>
-      <c r="S6" s="38">
+      <c r="R6" s="32">
+        <v>0</v>
+      </c>
+      <c r="S6" s="32">
         <v>2</v>
       </c>
-      <c r="T6" s="38">
-        <v>0</v>
-      </c>
-      <c r="U6" s="38">
-        <v>0</v>
-      </c>
-      <c r="V6" s="38">
-        <v>0</v>
-      </c>
-      <c r="W6" s="38">
-        <v>0</v>
-      </c>
-      <c r="X6" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="39">
+      <c r="T6" s="32">
+        <v>0</v>
+      </c>
+      <c r="U6" s="32">
+        <v>0</v>
+      </c>
+      <c r="V6" s="32">
+        <v>0</v>
+      </c>
+      <c r="W6" s="32">
+        <v>0</v>
+      </c>
+      <c r="X6" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="33">
         <v>0</v>
       </c>
     </row>
@@ -12098,88 +12485,88 @@
       <c r="A7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="44">
-        <v>1</v>
-      </c>
-      <c r="C7" s="45">
-        <v>0</v>
-      </c>
-      <c r="D7" s="45">
-        <v>0</v>
-      </c>
-      <c r="E7" s="45">
-        <v>0</v>
-      </c>
-      <c r="F7" s="45">
-        <v>0</v>
-      </c>
-      <c r="G7" s="45">
-        <v>0</v>
-      </c>
-      <c r="H7" s="45">
-        <v>0</v>
-      </c>
-      <c r="I7" s="45">
-        <v>0</v>
-      </c>
-      <c r="J7" s="45">
-        <v>0</v>
-      </c>
-      <c r="K7" s="45">
-        <v>0</v>
-      </c>
-      <c r="L7" s="45">
-        <v>0</v>
-      </c>
-      <c r="M7" s="45">
-        <v>0</v>
-      </c>
-      <c r="N7" s="45">
-        <v>0</v>
-      </c>
-      <c r="O7" s="45">
-        <v>0</v>
-      </c>
-      <c r="P7" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="45">
-        <v>0</v>
-      </c>
-      <c r="R7" s="45">
-        <v>0</v>
-      </c>
-      <c r="S7" s="45">
-        <v>0</v>
-      </c>
-      <c r="T7" s="45">
-        <v>0</v>
-      </c>
-      <c r="U7" s="45">
-        <v>0</v>
-      </c>
-      <c r="V7" s="45">
-        <v>0</v>
-      </c>
-      <c r="W7" s="45">
-        <v>0</v>
-      </c>
-      <c r="X7" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="40">
+      <c r="B7" s="38">
+        <v>1</v>
+      </c>
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
+      <c r="D7" s="39">
+        <v>0</v>
+      </c>
+      <c r="E7" s="39">
+        <v>0</v>
+      </c>
+      <c r="F7" s="39">
+        <v>0</v>
+      </c>
+      <c r="G7" s="39">
+        <v>0</v>
+      </c>
+      <c r="H7" s="39">
+        <v>0</v>
+      </c>
+      <c r="I7" s="39">
+        <v>0</v>
+      </c>
+      <c r="J7" s="39">
+        <v>0</v>
+      </c>
+      <c r="K7" s="39">
+        <v>0</v>
+      </c>
+      <c r="L7" s="39">
+        <v>0</v>
+      </c>
+      <c r="M7" s="39">
+        <v>0</v>
+      </c>
+      <c r="N7" s="39">
+        <v>0</v>
+      </c>
+      <c r="O7" s="39">
+        <v>0</v>
+      </c>
+      <c r="P7" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="39">
+        <v>0</v>
+      </c>
+      <c r="R7" s="39">
+        <v>0</v>
+      </c>
+      <c r="S7" s="39">
+        <v>0</v>
+      </c>
+      <c r="T7" s="39">
+        <v>0</v>
+      </c>
+      <c r="U7" s="39">
+        <v>0</v>
+      </c>
+      <c r="V7" s="39">
+        <v>0</v>
+      </c>
+      <c r="W7" s="39">
+        <v>0</v>
+      </c>
+      <c r="X7" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="39">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="34">
         <v>0</v>
       </c>
     </row>
@@ -12187,88 +12574,88 @@
       <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="38">
         <v>2</v>
       </c>
-      <c r="C8" s="45">
-        <v>0</v>
-      </c>
-      <c r="D8" s="46">
+      <c r="C8" s="39">
+        <v>0</v>
+      </c>
+      <c r="D8" s="40">
         <v>2</v>
       </c>
-      <c r="E8" s="45">
-        <v>0</v>
-      </c>
-      <c r="F8" s="45">
-        <v>0</v>
-      </c>
-      <c r="G8" s="45">
-        <v>0</v>
-      </c>
-      <c r="H8" s="46">
+      <c r="E8" s="39">
+        <v>0</v>
+      </c>
+      <c r="F8" s="39">
+        <v>0</v>
+      </c>
+      <c r="G8" s="39">
+        <v>0</v>
+      </c>
+      <c r="H8" s="40">
         <v>2</v>
       </c>
-      <c r="I8" s="45">
-        <v>0</v>
-      </c>
-      <c r="J8" s="45">
-        <v>0</v>
-      </c>
-      <c r="K8" s="46">
+      <c r="I8" s="39">
+        <v>0</v>
+      </c>
+      <c r="J8" s="39">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
         <v>2</v>
       </c>
-      <c r="L8" s="45">
-        <v>0</v>
-      </c>
-      <c r="M8" s="45">
-        <v>0</v>
-      </c>
-      <c r="N8" s="45">
-        <v>0</v>
-      </c>
-      <c r="O8" s="46">
+      <c r="L8" s="39">
+        <v>0</v>
+      </c>
+      <c r="M8" s="39">
+        <v>0</v>
+      </c>
+      <c r="N8" s="39">
+        <v>0</v>
+      </c>
+      <c r="O8" s="40">
         <v>2</v>
       </c>
-      <c r="P8" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="45">
-        <v>0</v>
-      </c>
-      <c r="R8" s="46">
+      <c r="P8" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="39">
+        <v>0</v>
+      </c>
+      <c r="R8" s="40">
         <v>2</v>
       </c>
-      <c r="S8" s="45">
-        <v>0</v>
-      </c>
-      <c r="T8" s="45">
-        <v>0</v>
-      </c>
-      <c r="U8" s="45">
-        <v>0</v>
-      </c>
-      <c r="V8" s="46">
+      <c r="S8" s="39">
+        <v>0</v>
+      </c>
+      <c r="T8" s="39">
+        <v>0</v>
+      </c>
+      <c r="U8" s="39">
+        <v>0</v>
+      </c>
+      <c r="V8" s="40">
         <v>2</v>
       </c>
-      <c r="W8" s="46">
+      <c r="W8" s="40">
         <v>2</v>
       </c>
-      <c r="X8" s="46">
+      <c r="X8" s="40">
         <v>2</v>
       </c>
-      <c r="Y8" s="46">
+      <c r="Y8" s="40">
         <v>2</v>
       </c>
-      <c r="Z8" s="46">
+      <c r="Z8" s="40">
         <v>2</v>
       </c>
-      <c r="AA8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="40">
+      <c r="AA8" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="34">
         <v>0</v>
       </c>
     </row>
@@ -12276,88 +12663,88 @@
       <c r="A9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="43">
-        <v>0</v>
-      </c>
-      <c r="C9" s="38">
-        <v>0</v>
-      </c>
-      <c r="D9" s="38">
-        <v>1</v>
-      </c>
-      <c r="E9" s="38">
-        <v>0</v>
-      </c>
-      <c r="F9" s="38">
-        <v>1</v>
-      </c>
-      <c r="G9" s="38">
-        <v>0</v>
-      </c>
-      <c r="H9" s="38">
-        <v>0</v>
-      </c>
-      <c r="I9" s="38">
-        <v>0</v>
-      </c>
-      <c r="J9" s="38">
-        <v>0</v>
-      </c>
-      <c r="K9" s="38">
-        <v>0</v>
-      </c>
-      <c r="L9" s="38">
-        <v>1</v>
-      </c>
-      <c r="M9" s="38">
-        <v>0</v>
-      </c>
-      <c r="N9" s="38">
-        <v>0</v>
-      </c>
-      <c r="O9" s="38">
-        <v>0</v>
-      </c>
-      <c r="P9" s="38">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="38">
-        <v>0</v>
-      </c>
-      <c r="R9" s="38">
-        <v>0</v>
-      </c>
-      <c r="S9" s="38">
-        <v>0</v>
-      </c>
-      <c r="T9" s="38">
-        <v>0</v>
-      </c>
-      <c r="U9" s="38">
-        <v>0</v>
-      </c>
-      <c r="V9" s="38">
-        <v>0</v>
-      </c>
-      <c r="W9" s="38">
-        <v>0</v>
-      </c>
-      <c r="X9" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="38">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="38">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="38">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="39">
+      <c r="B9" s="37">
+        <v>0</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0</v>
+      </c>
+      <c r="D9" s="32">
+        <v>1</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="32">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0</v>
+      </c>
+      <c r="J9" s="32">
+        <v>0</v>
+      </c>
+      <c r="K9" s="32">
+        <v>0</v>
+      </c>
+      <c r="L9" s="32">
+        <v>1</v>
+      </c>
+      <c r="M9" s="32">
+        <v>0</v>
+      </c>
+      <c r="N9" s="32">
+        <v>0</v>
+      </c>
+      <c r="O9" s="32">
+        <v>0</v>
+      </c>
+      <c r="P9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="32">
+        <v>0</v>
+      </c>
+      <c r="R9" s="32">
+        <v>0</v>
+      </c>
+      <c r="S9" s="32">
+        <v>0</v>
+      </c>
+      <c r="T9" s="32">
+        <v>0</v>
+      </c>
+      <c r="U9" s="32">
+        <v>0</v>
+      </c>
+      <c r="V9" s="32">
+        <v>0</v>
+      </c>
+      <c r="W9" s="32">
+        <v>0</v>
+      </c>
+      <c r="X9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="32">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="33">
         <v>0</v>
       </c>
     </row>
@@ -12365,88 +12752,88 @@
       <c r="A10" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="47">
-        <v>0</v>
-      </c>
-      <c r="C10" s="48">
-        <v>0</v>
-      </c>
-      <c r="D10" s="48">
-        <v>0</v>
-      </c>
-      <c r="E10" s="48">
-        <v>0</v>
-      </c>
-      <c r="F10" s="48">
-        <v>1</v>
-      </c>
-      <c r="G10" s="41">
-        <v>0</v>
-      </c>
-      <c r="H10" s="41">
-        <v>0</v>
-      </c>
-      <c r="I10" s="41">
-        <v>0</v>
-      </c>
-      <c r="J10" s="41">
-        <v>0</v>
-      </c>
-      <c r="K10" s="41">
-        <v>0</v>
-      </c>
-      <c r="L10" s="41">
-        <v>0</v>
-      </c>
-      <c r="M10" s="41">
-        <v>0</v>
-      </c>
-      <c r="N10" s="41">
-        <v>0</v>
-      </c>
-      <c r="O10" s="41">
-        <v>0</v>
-      </c>
-      <c r="P10" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="41">
-        <v>0</v>
-      </c>
-      <c r="R10" s="41">
-        <v>0</v>
-      </c>
-      <c r="S10" s="41">
-        <v>0</v>
-      </c>
-      <c r="T10" s="41">
-        <v>0</v>
-      </c>
-      <c r="U10" s="41">
-        <v>0</v>
-      </c>
-      <c r="V10" s="41">
-        <v>0</v>
-      </c>
-      <c r="W10" s="41">
-        <v>0</v>
-      </c>
-      <c r="X10" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="41">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="41">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="49">
+      <c r="B10" s="41">
+        <v>0</v>
+      </c>
+      <c r="C10" s="42">
+        <v>0</v>
+      </c>
+      <c r="D10" s="42">
+        <v>0</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+      <c r="F10" s="42">
+        <v>1</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0</v>
+      </c>
+      <c r="H10" s="35">
+        <v>0</v>
+      </c>
+      <c r="I10" s="35">
+        <v>0</v>
+      </c>
+      <c r="J10" s="35">
+        <v>0</v>
+      </c>
+      <c r="K10" s="35">
+        <v>0</v>
+      </c>
+      <c r="L10" s="35">
+        <v>0</v>
+      </c>
+      <c r="M10" s="35">
+        <v>0</v>
+      </c>
+      <c r="N10" s="35">
+        <v>0</v>
+      </c>
+      <c r="O10" s="35">
+        <v>0</v>
+      </c>
+      <c r="P10" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="35">
+        <v>0</v>
+      </c>
+      <c r="R10" s="35">
+        <v>0</v>
+      </c>
+      <c r="S10" s="35">
+        <v>0</v>
+      </c>
+      <c r="T10" s="35">
+        <v>0</v>
+      </c>
+      <c r="U10" s="35">
+        <v>0</v>
+      </c>
+      <c r="V10" s="35">
+        <v>0</v>
+      </c>
+      <c r="W10" s="35">
+        <v>0</v>
+      </c>
+      <c r="X10" s="35">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="35">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="35">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="35">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="35">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="43">
         <v>0</v>
       </c>
     </row>
@@ -12454,88 +12841,88 @@
       <c r="A11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="50">
-        <v>0</v>
-      </c>
-      <c r="C11" s="46">
-        <v>1</v>
-      </c>
-      <c r="D11" s="45">
-        <v>0</v>
-      </c>
-      <c r="E11" s="45">
-        <v>0</v>
-      </c>
-      <c r="F11" s="46">
-        <v>1</v>
-      </c>
-      <c r="G11" s="45">
-        <v>0</v>
-      </c>
-      <c r="H11" s="45">
-        <v>0</v>
-      </c>
-      <c r="I11" s="45">
-        <v>0</v>
-      </c>
-      <c r="J11" s="45">
-        <v>0</v>
-      </c>
-      <c r="K11" s="45">
-        <v>0</v>
-      </c>
-      <c r="L11" s="45">
-        <v>0</v>
-      </c>
-      <c r="M11" s="46">
-        <v>1</v>
-      </c>
-      <c r="N11" s="45">
-        <v>0</v>
-      </c>
-      <c r="O11" s="45">
-        <v>0</v>
-      </c>
-      <c r="P11" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="45">
-        <v>0</v>
-      </c>
-      <c r="R11" s="45">
-        <v>0</v>
-      </c>
-      <c r="S11" s="45">
-        <v>0</v>
-      </c>
-      <c r="T11" s="45">
-        <v>0</v>
-      </c>
-      <c r="U11" s="45">
-        <v>0</v>
-      </c>
-      <c r="V11" s="45">
-        <v>0</v>
-      </c>
-      <c r="W11" s="45">
-        <v>0</v>
-      </c>
-      <c r="X11" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="46">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="40">
+      <c r="B11" s="44">
+        <v>0</v>
+      </c>
+      <c r="C11" s="40">
+        <v>1</v>
+      </c>
+      <c r="D11" s="39">
+        <v>0</v>
+      </c>
+      <c r="E11" s="39">
+        <v>0</v>
+      </c>
+      <c r="F11" s="40">
+        <v>1</v>
+      </c>
+      <c r="G11" s="39">
+        <v>0</v>
+      </c>
+      <c r="H11" s="39">
+        <v>0</v>
+      </c>
+      <c r="I11" s="39">
+        <v>0</v>
+      </c>
+      <c r="J11" s="39">
+        <v>0</v>
+      </c>
+      <c r="K11" s="39">
+        <v>0</v>
+      </c>
+      <c r="L11" s="39">
+        <v>0</v>
+      </c>
+      <c r="M11" s="40">
+        <v>1</v>
+      </c>
+      <c r="N11" s="39">
+        <v>0</v>
+      </c>
+      <c r="O11" s="39">
+        <v>0</v>
+      </c>
+      <c r="P11" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="39">
+        <v>0</v>
+      </c>
+      <c r="R11" s="39">
+        <v>0</v>
+      </c>
+      <c r="S11" s="39">
+        <v>0</v>
+      </c>
+      <c r="T11" s="39">
+        <v>0</v>
+      </c>
+      <c r="U11" s="39">
+        <v>0</v>
+      </c>
+      <c r="V11" s="39">
+        <v>0</v>
+      </c>
+      <c r="W11" s="39">
+        <v>0</v>
+      </c>
+      <c r="X11" s="39">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="39">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="40">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="39">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="34">
         <v>0</v>
       </c>
     </row>
@@ -12543,88 +12930,88 @@
       <c r="A12" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="47">
-        <v>0</v>
-      </c>
-      <c r="C12" s="48">
-        <v>1</v>
-      </c>
-      <c r="D12" s="48">
-        <v>0</v>
-      </c>
-      <c r="E12" s="48">
-        <v>0</v>
-      </c>
-      <c r="F12" s="48">
-        <v>1</v>
-      </c>
-      <c r="G12" s="45">
-        <v>1</v>
-      </c>
-      <c r="H12" s="48">
-        <v>0</v>
-      </c>
-      <c r="I12" s="48">
-        <v>0</v>
-      </c>
-      <c r="J12" s="48">
-        <v>0</v>
-      </c>
-      <c r="K12" s="48">
-        <v>0</v>
-      </c>
-      <c r="L12" s="48">
-        <v>0</v>
-      </c>
-      <c r="M12" s="48">
-        <v>1</v>
-      </c>
-      <c r="N12" s="45">
+      <c r="B12" s="41">
+        <v>0</v>
+      </c>
+      <c r="C12" s="42">
+        <v>1</v>
+      </c>
+      <c r="D12" s="42">
+        <v>0</v>
+      </c>
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+      <c r="F12" s="42">
+        <v>1</v>
+      </c>
+      <c r="G12" s="39">
+        <v>1</v>
+      </c>
+      <c r="H12" s="42">
+        <v>0</v>
+      </c>
+      <c r="I12" s="42">
+        <v>0</v>
+      </c>
+      <c r="J12" s="42">
+        <v>0</v>
+      </c>
+      <c r="K12" s="42">
+        <v>0</v>
+      </c>
+      <c r="L12" s="42">
+        <v>0</v>
+      </c>
+      <c r="M12" s="42">
+        <v>1</v>
+      </c>
+      <c r="N12" s="39">
         <v>2</v>
       </c>
-      <c r="O12" s="48">
-        <v>0</v>
-      </c>
-      <c r="P12" s="48">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="48">
-        <v>0</v>
-      </c>
-      <c r="R12" s="48">
-        <v>0</v>
-      </c>
-      <c r="S12" s="48">
-        <v>0</v>
-      </c>
-      <c r="T12" s="48">
-        <v>0</v>
-      </c>
-      <c r="U12" s="48">
-        <v>0</v>
-      </c>
-      <c r="V12" s="48">
-        <v>0</v>
-      </c>
-      <c r="W12" s="48">
-        <v>0</v>
-      </c>
-      <c r="X12" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="48">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="48">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="48">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="48">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="51">
+      <c r="O12" s="42">
+        <v>0</v>
+      </c>
+      <c r="P12" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="42">
+        <v>0</v>
+      </c>
+      <c r="R12" s="42">
+        <v>0</v>
+      </c>
+      <c r="S12" s="42">
+        <v>0</v>
+      </c>
+      <c r="T12" s="42">
+        <v>0</v>
+      </c>
+      <c r="U12" s="42">
+        <v>0</v>
+      </c>
+      <c r="V12" s="42">
+        <v>0</v>
+      </c>
+      <c r="W12" s="42">
+        <v>0</v>
+      </c>
+      <c r="X12" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="42">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="42">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="42">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="45">
         <v>0</v>
       </c>
     </row>
@@ -12632,7 +13019,7 @@
       <c r="A13" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="46">
         <v>3</v>
       </c>
       <c r="C13" s="26">
@@ -12721,7 +13108,7 @@
       <c r="A14" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B14" s="47">
         <v>1</v>
       </c>
       <c r="C14" s="30">
@@ -12928,6 +13315,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -12936,102 +13324,102 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="57" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="57"/>
+    <col min="1" max="1" width="15.83203125" style="51" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="51"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="60" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="52">
+        <v>5</v>
+      </c>
+      <c r="C3" s="52">
+        <v>0</v>
+      </c>
+      <c r="D3" s="52">
         <v>4</v>
       </c>
-      <c r="C3" s="58">
-        <v>0</v>
-      </c>
-      <c r="D3" s="58">
-        <v>4</v>
-      </c>
-      <c r="E3" s="58">
-        <v>1</v>
-      </c>
-      <c r="F3" s="59">
+      <c r="E3" s="52">
+        <v>1</v>
+      </c>
+      <c r="F3" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="58">
-        <v>0</v>
-      </c>
-      <c r="C4" s="58">
-        <v>1</v>
-      </c>
-      <c r="D4" s="58">
+      <c r="B4" s="52">
+        <v>0</v>
+      </c>
+      <c r="C4" s="52">
+        <v>1</v>
+      </c>
+      <c r="D4" s="52">
         <v>2</v>
       </c>
-      <c r="E4" s="58">
-        <v>1</v>
-      </c>
-      <c r="F4" s="59">
+      <c r="E4" s="52">
+        <v>1</v>
+      </c>
+      <c r="F4" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="54">
         <v>4</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="54">
         <v>2</v>
       </c>
-      <c r="D5" s="60">
-        <v>1</v>
-      </c>
-      <c r="E5" s="60">
-        <v>0</v>
-      </c>
-      <c r="F5" s="61">
+      <c r="D5" s="54">
+        <v>1</v>
+      </c>
+      <c r="E5" s="54">
+        <v>0</v>
+      </c>
+      <c r="F5" s="55">
         <v>2</v>
       </c>
     </row>
@@ -13047,5 +13435,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>